<commit_message>
response to reviewer edits
</commit_message>
<xml_diff>
--- a/Data/TRT_psi_notebook.xlsx
+++ b/Data/TRT_psi_notebook.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathanwood/Documents/GitHub/Split-Belt-AFC-Reliability/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC265031-3FF0-054A-966F-2DB3F02C2E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88883291-DFB3-1945-9B31-848FC49B3017}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20200" xr2:uid="{B99E37B8-408A-5F40-B244-1E4135A11673}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -288,7 +288,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -333,8 +333,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -660,7 +659,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -669,8 +668,7 @@
     <col min="2" max="2" width="14.83203125" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" style="14"/>
     <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="18"/>
-    <col min="7" max="8" width="10.83203125" style="19"/>
+    <col min="7" max="8" width="10.83203125" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -692,10 +690,10 @@
       <c r="F1" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="19" t="s">
         <v>33</v>
       </c>
     </row>
@@ -718,10 +716,10 @@
       <c r="F2" s="16">
         <v>31</v>
       </c>
-      <c r="G2" s="19">
+      <c r="G2" s="18">
         <v>-7</v>
       </c>
-      <c r="H2" s="19">
+      <c r="H2" s="18">
         <v>-6</v>
       </c>
     </row>
@@ -744,11 +742,11 @@
       <c r="F3" s="16">
         <v>22</v>
       </c>
-      <c r="G3" s="19">
-        <v>9</v>
-      </c>
-      <c r="H3" s="19">
-        <v>8</v>
+      <c r="G3" s="18">
+        <v>-9</v>
+      </c>
+      <c r="H3" s="18">
+        <v>-8</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -770,11 +768,11 @@
       <c r="F4" s="16">
         <v>23</v>
       </c>
-      <c r="G4" s="19">
-        <v>13</v>
-      </c>
-      <c r="H4" s="19">
-        <v>10</v>
+      <c r="G4" s="18">
+        <v>-13</v>
+      </c>
+      <c r="H4" s="18">
+        <v>-10</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -796,10 +794,10 @@
       <c r="F5" s="16">
         <v>23</v>
       </c>
-      <c r="G5" s="19">
+      <c r="G5" s="18">
         <v>0</v>
       </c>
-      <c r="H5" s="19">
+      <c r="H5" s="18">
         <v>-6</v>
       </c>
     </row>
@@ -822,11 +820,11 @@
       <c r="F6" s="16">
         <v>24</v>
       </c>
-      <c r="G6" s="19">
-        <v>14</v>
-      </c>
-      <c r="H6" s="19">
-        <v>12</v>
+      <c r="G6" s="18">
+        <v>-14</v>
+      </c>
+      <c r="H6" s="18">
+        <v>-12</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -848,10 +846,10 @@
       <c r="F7" s="16">
         <v>32</v>
       </c>
-      <c r="G7" s="19">
+      <c r="G7" s="18">
         <v>33</v>
       </c>
-      <c r="H7" s="19">
+      <c r="H7" s="18">
         <v>29</v>
       </c>
     </row>
@@ -874,10 +872,10 @@
       <c r="F8" s="16">
         <v>26</v>
       </c>
-      <c r="G8" s="19">
+      <c r="G8" s="18">
         <v>-13</v>
       </c>
-      <c r="H8" s="19">
+      <c r="H8" s="18">
         <v>-18</v>
       </c>
     </row>
@@ -900,10 +898,10 @@
       <c r="F9" s="16">
         <v>20</v>
       </c>
-      <c r="G9" s="19">
+      <c r="G9" s="18">
         <v>-1</v>
       </c>
-      <c r="H9" s="19">
+      <c r="H9" s="18">
         <v>6</v>
       </c>
     </row>
@@ -926,11 +924,11 @@
       <c r="F10" s="16">
         <v>18</v>
       </c>
-      <c r="G10" s="19">
-        <v>14</v>
-      </c>
-      <c r="H10" s="19">
-        <v>12</v>
+      <c r="G10" s="18">
+        <v>-14</v>
+      </c>
+      <c r="H10" s="18">
+        <v>-12</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -952,10 +950,10 @@
       <c r="F11" s="17">
         <v>21</v>
       </c>
-      <c r="G11" s="21">
+      <c r="G11" s="20">
         <v>23</v>
       </c>
-      <c r="H11" s="21">
+      <c r="H11" s="20">
         <v>22</v>
       </c>
     </row>
@@ -978,10 +976,10 @@
       <c r="F12" s="16">
         <v>26</v>
       </c>
-      <c r="G12" s="19">
+      <c r="G12" s="18">
         <v>21</v>
       </c>
-      <c r="H12" s="19">
+      <c r="H12" s="18">
         <v>13</v>
       </c>
     </row>
@@ -1004,10 +1002,10 @@
       <c r="F13" s="16">
         <v>22</v>
       </c>
-      <c r="G13" s="19">
+      <c r="G13" s="18">
         <v>4</v>
       </c>
-      <c r="H13" s="19">
+      <c r="H13" s="18">
         <v>9</v>
       </c>
     </row>
@@ -1030,10 +1028,10 @@
       <c r="F14" s="16">
         <v>24</v>
       </c>
-      <c r="G14" s="19">
+      <c r="G14" s="18">
         <v>35</v>
       </c>
-      <c r="H14" s="19">
+      <c r="H14" s="18">
         <v>47</v>
       </c>
     </row>
@@ -1056,10 +1054,10 @@
       <c r="F15" s="16">
         <v>21</v>
       </c>
-      <c r="G15" s="19">
+      <c r="G15" s="18">
         <v>15</v>
       </c>
-      <c r="H15" s="19">
+      <c r="H15" s="18">
         <v>28</v>
       </c>
     </row>
@@ -1082,10 +1080,10 @@
       <c r="F16" s="16">
         <v>30</v>
       </c>
-      <c r="G16" s="19">
+      <c r="G16" s="18">
         <v>-5</v>
       </c>
-      <c r="H16" s="19">
+      <c r="H16" s="18">
         <v>-4</v>
       </c>
     </row>
@@ -1108,10 +1106,10 @@
       <c r="F17" s="16">
         <v>23</v>
       </c>
-      <c r="G17" s="19">
+      <c r="G17" s="18">
         <v>13</v>
       </c>
-      <c r="H17" s="19">
+      <c r="H17" s="18">
         <v>24</v>
       </c>
     </row>
@@ -1134,10 +1132,10 @@
       <c r="F18" s="16">
         <v>20</v>
       </c>
-      <c r="G18" s="19">
+      <c r="G18" s="18">
         <v>-2</v>
       </c>
-      <c r="H18" s="19">
+      <c r="H18" s="18">
         <v>4</v>
       </c>
     </row>
@@ -1160,10 +1158,10 @@
       <c r="F19" s="16">
         <v>23</v>
       </c>
-      <c r="G19" s="19">
+      <c r="G19" s="18">
         <v>-8</v>
       </c>
-      <c r="H19" s="19">
+      <c r="H19" s="18">
         <v>2</v>
       </c>
     </row>
@@ -1186,10 +1184,10 @@
       <c r="F20" s="16">
         <v>27</v>
       </c>
-      <c r="G20" s="19">
+      <c r="G20" s="18">
         <v>32</v>
       </c>
-      <c r="H20" s="19">
+      <c r="H20" s="18">
         <v>32</v>
       </c>
     </row>
@@ -1212,10 +1210,10 @@
       <c r="F21" s="16">
         <v>18</v>
       </c>
-      <c r="G21" s="19">
+      <c r="G21" s="18">
         <v>29</v>
       </c>
-      <c r="H21" s="19">
+      <c r="H21" s="18">
         <v>19</v>
       </c>
     </row>
@@ -1238,10 +1236,10 @@
       <c r="F22" s="16">
         <v>23</v>
       </c>
-      <c r="G22" s="19">
+      <c r="G22" s="18">
         <v>16</v>
       </c>
-      <c r="H22" s="19">
+      <c r="H22" s="18">
         <v>32</v>
       </c>
     </row>
@@ -1264,10 +1262,10 @@
       <c r="F23" s="16">
         <v>19</v>
       </c>
-      <c r="G23" s="19">
+      <c r="G23" s="18">
         <v>10</v>
       </c>
-      <c r="H23" s="19">
+      <c r="H23" s="18">
         <v>-6</v>
       </c>
     </row>
@@ -1290,10 +1288,10 @@
       <c r="F24" s="12">
         <v>19</v>
       </c>
-      <c r="G24" s="19">
+      <c r="G24" s="18">
         <v>-2</v>
       </c>
-      <c r="H24" s="19">
+      <c r="H24" s="18">
         <v>0</v>
       </c>
     </row>

</xml_diff>